<commit_message>
hours and top 500 started
</commit_message>
<xml_diff>
--- a/admin/Kate_and_Ben_hours.xlsx
+++ b/admin/Kate_and_Ben_hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/benjamin_millard-martin_mail_mcgill_ca/Documents/Documents/eDNA Thesis/repos/GAPP/admin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katesheridan/Documents/GitHub/GAPP/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{6C7139FF-0C22-468C-B9BC-E3844028A604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE623622-2A94-4099-9204-C3869991D436}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCFF9B5-66BC-3A4A-9C65-CE4DFE791BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="552" windowWidth="21636" windowHeight="11256" activeTab="1" xr2:uid="{11ACFB21-8D2F-4C96-80F1-719252D4D08A}"/>
+    <workbookView xWindow="38400" yWindow="1000" windowWidth="22540" windowHeight="14880" xr2:uid="{11ACFB21-8D2F-4C96-80F1-719252D4D08A}"/>
   </bookViews>
   <sheets>
     <sheet name="Kate_hours" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>meeting with Kate, taxonomy script, research database coverage approach</t>
+  </si>
+  <si>
+    <t>Meet with Ben, Jenn, and Eden</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Ben and Kate meeting to discuss workflow and assign tasks, OBIS download + initial cleaning</t>
+  </si>
+  <si>
+    <t>GBIF setup and prepping species lists</t>
+  </si>
+  <si>
+    <t>Met with Ben, updated OBIS for ecoregions</t>
+  </si>
+  <si>
+    <t>Fixed loop, top 500 taxize</t>
   </si>
 </sst>
 </file>
@@ -99,9 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,10 +136,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,19 +435,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC32E3D-3FDD-49CE-BA1E-985B1B05C4DC}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,6 +456,92 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>44998</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>45005</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45014</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45015</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>45020</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>45028</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <f>SUM(B2:B27)</f>
+        <v>24.5</v>
       </c>
     </row>
   </sheetData>
@@ -452,18 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E08762-4695-4E9C-B049-542E7025AD67}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="74.21875" customWidth="1"/>
+    <col min="3" max="3" width="74.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44998</v>
       </c>
@@ -485,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45005</v>
       </c>
@@ -496,7 +597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45014</v>
       </c>
@@ -507,7 +608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45020</v>
       </c>
@@ -518,7 +619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45021</v>
       </c>
@@ -529,7 +630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>45026</v>
       </c>
@@ -540,7 +641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>45027</v>
       </c>

</xml_diff>

<commit_message>
documentation + fishbase validation rolled in
</commit_message>
<xml_diff>
--- a/admin/Kate_and_Ben_hours.xlsx
+++ b/admin/Kate_and_Ben_hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/benjamin_millard-martin_mail_mcgill_ca/Documents/Documents/eDNA Thesis/repos/GAPP/admin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katesheridan/Documents/GitHub/GAPP/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{9BCFF9B5-66BC-3A4A-9C65-CE4DFE791BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6D71939-3A8B-424D-B2C8-68C51FC5F7D6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C8EC21-7AC1-8D4C-8CC4-C2FF0B336038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="30555" yWindow="1410" windowWidth="27045" windowHeight="14070" activeTab="1" xr2:uid="{11ACFB21-8D2F-4C96-80F1-719252D4D08A}"/>
+    <workbookView xWindow="9140" yWindow="600" windowWidth="27040" windowHeight="14080" xr2:uid="{11ACFB21-8D2F-4C96-80F1-719252D4D08A}"/>
   </bookViews>
   <sheets>
     <sheet name="Kate_hours" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>Python, BLAST seach, outut</t>
+  </si>
+  <si>
+    <t>set up worms records search, taxonomy</t>
+  </si>
+  <si>
+    <t>comparison lists, region setup transferred</t>
+  </si>
+  <si>
+    <t>documentation, helping</t>
+  </si>
+  <si>
+    <t>meeting about goals</t>
+  </si>
+  <si>
+    <t>workflow planning</t>
   </si>
 </sst>
 </file>
@@ -148,10 +163,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -453,17 +464,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC32E3D-3FDD-49CE-BA1E-985B1B05C4DC}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44998</v>
       </c>
@@ -485,7 +496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45005</v>
       </c>
@@ -496,7 +507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45014</v>
       </c>
@@ -507,7 +518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45015</v>
       </c>
@@ -518,7 +529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45020</v>
       </c>
@@ -529,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45027</v>
       </c>
@@ -540,7 +551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45028</v>
       </c>
@@ -551,13 +562,68 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>45029</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>45034</v>
+      </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>45036</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>45037</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>10</v>
       </c>
       <c r="B29">
         <f>SUM(B2:B27)</f>
-        <v>24.5</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -569,18 +635,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E08762-4695-4E9C-B049-542E7025AD67}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="74.109375" customWidth="1"/>
+    <col min="3" max="3" width="74.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44998</v>
       </c>
@@ -602,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45005</v>
       </c>
@@ -613,7 +679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45014</v>
       </c>
@@ -624,7 +690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45020</v>
       </c>
@@ -635,7 +701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45021</v>
       </c>
@@ -646,7 +712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>45026</v>
       </c>
@@ -657,7 +723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>45027</v>
       </c>
@@ -668,7 +734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>45028</v>
       </c>
@@ -679,7 +745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>45029</v>
       </c>
@@ -690,7 +756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>45030</v>
       </c>
@@ -701,7 +767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>45033</v>
       </c>
@@ -712,7 +778,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>45036</v>
       </c>
@@ -723,7 +789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>45037</v>
       </c>
@@ -734,7 +800,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>45040</v>
       </c>
@@ -745,7 +811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27">
         <f>SUM(B2:B15)</f>
         <v>61.5</v>

</xml_diff>

<commit_message>
ncbi search set up
</commit_message>
<xml_diff>
--- a/admin/Kate_and_Ben_hours.xlsx
+++ b/admin/Kate_and_Ben_hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/benjamin_millard-martin_mail_mcgill_ca/Documents/Documents/eDNA Thesis/repos/GAPP/admin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katesheridan/Documents/GitHub/GAPP/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F7DA0E41-6230-9A43-A4EC-C12CEE4AA001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7D9D33D-3E86-4B33-896A-F6E6AE363605}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC2BBA6-3ABC-4340-A94F-1838A59ECD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{11ACFB21-8D2F-4C96-80F1-719252D4D08A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{11ACFB21-8D2F-4C96-80F1-719252D4D08A}"/>
   </bookViews>
   <sheets>
     <sheet name="Kate_hours" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>sum(</t>
+  </si>
+  <si>
+    <t>docmentation, fixing past scripts, updated outputs</t>
   </si>
 </sst>
 </file>
@@ -476,17 +479,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC32E3D-3FDD-49CE-BA1E-985B1B05C4DC}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44998</v>
       </c>
@@ -508,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45005</v>
       </c>
@@ -519,7 +522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45014</v>
       </c>
@@ -530,7 +533,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45015</v>
       </c>
@@ -541,7 +544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45020</v>
       </c>
@@ -552,7 +555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45027</v>
       </c>
@@ -563,7 +566,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45028</v>
       </c>
@@ -574,7 +577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45029</v>
       </c>
@@ -585,7 +588,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45030</v>
       </c>
@@ -596,7 +599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>45034</v>
       </c>
@@ -607,7 +610,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45036</v>
       </c>
@@ -618,7 +621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45037</v>
       </c>
@@ -629,7 +632,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>45044</v>
       </c>
@@ -640,13 +643,24 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>45047</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>10</v>
       </c>
       <c r="B29">
         <f>SUM(B2:B27)</f>
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -658,18 +672,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E08762-4695-4E9C-B049-542E7025AD67}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="74.109375" customWidth="1"/>
+    <col min="3" max="3" width="74.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44998</v>
       </c>
@@ -691,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45005</v>
       </c>
@@ -702,7 +716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45014</v>
       </c>
@@ -713,7 +727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45020</v>
       </c>
@@ -724,7 +738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45021</v>
       </c>
@@ -735,7 +749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>45026</v>
       </c>
@@ -746,7 +760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>45027</v>
       </c>
@@ -757,7 +771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>45028</v>
       </c>
@@ -768,7 +782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>45029</v>
       </c>
@@ -779,7 +793,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>45030</v>
       </c>
@@ -790,7 +804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>45033</v>
       </c>
@@ -801,7 +815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>45036</v>
       </c>
@@ -812,7 +826,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>45037</v>
       </c>
@@ -823,7 +837,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>45040</v>
       </c>
@@ -834,7 +848,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>45041</v>
       </c>
@@ -845,7 +859,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>45043</v>
       </c>
@@ -856,7 +870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>45047</v>
       </c>
@@ -867,7 +881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>27</v>
       </c>

</xml_diff>